<commit_message>
le monstre et la fille
</commit_message>
<xml_diff>
--- a/musiques.xlsx
+++ b/musiques.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="1308" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="3708" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="111" uniqueCount="111">
   <si>
     <t>army of doom</t>
   </si>
@@ -308,6 +308,45 @@
   </si>
   <si>
     <t>https://www.youtube.com/watch?v=z4-6Shvg8js</t>
+  </si>
+  <si>
+    <t>regard en arrierre</t>
+  </si>
+  <si>
+    <t>Epilogue : beginning</t>
+  </si>
+  <si>
+    <t>Faded snapshots and forgotten dreams</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=TYevEJ6y7Uo</t>
+  </si>
+  <si>
+    <t>regard en avant</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=08XIghnIjWs</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=Tzu8gBR0joY</t>
+  </si>
+  <si>
+    <t>final conclusion</t>
+  </si>
+  <si>
+    <t>One dark mare</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=GfXAojf56wg</t>
+  </si>
+  <si>
+    <t>Sophia</t>
+  </si>
+  <si>
+    <t>posthumain</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=cOSAl26hyBQ</t>
   </si>
 </sst>
 </file>
@@ -376,9 +415,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:J46" totalsRowShown="0">
-  <autoFilter ref="A1:J46"/>
-  <tableColumns count="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:M50" totalsRowShown="0">
+  <autoFilter ref="A1:M50"/>
+  <tableColumns count="13">
     <tableColumn id="1" name="titre"/>
     <tableColumn id="7" name="Lien"/>
     <tableColumn id="2" name="dark"/>
@@ -389,6 +428,9 @@
     <tableColumn id="8" name="perturbant"/>
     <tableColumn id="9" name="aventure"/>
     <tableColumn id="10" name="mysterieux"/>
+    <tableColumn id="12" name="regard en arrierre"/>
+    <tableColumn id="13" name="regard en avant"/>
+    <tableColumn id="11" name="posthumain"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -681,23 +723,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J45"/>
+  <dimension ref="A1:M50"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A34" workbookViewId="0">
-      <selection activeCell="D8" sqref="D8"/>
+    <sheetView tabSelected="1" topLeftCell="A31" workbookViewId="0">
+      <selection activeCell="M43" sqref="M43"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="2" width="25.6640625" customWidth="1"/>
+    <col min="1" max="1" width="34.33203125" customWidth="1"/>
+    <col min="2" max="2" width="7" customWidth="1"/>
     <col min="5" max="5" width="13.21875" customWidth="1"/>
     <col min="7" max="7" width="10.44140625" customWidth="1"/>
     <col min="8" max="8" width="11.5546875" customWidth="1"/>
     <col min="9" max="9" width="10.109375" customWidth="1"/>
     <col min="10" max="10" width="11.5546875" customWidth="1"/>
+    <col min="11" max="11" width="18.77734375" customWidth="1"/>
+    <col min="12" max="12" width="16.6640625" customWidth="1"/>
+    <col min="13" max="13" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A1" t="s">
         <v>53</v>
       </c>
@@ -728,8 +774,17 @@
       <c r="J1" t="s">
         <v>51</v>
       </c>
-    </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K1" t="s">
+        <v>98</v>
+      </c>
+      <c r="L1" t="s">
+        <v>102</v>
+      </c>
+      <c r="M1" t="s">
+        <v>109</v>
+      </c>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -760,8 +815,14 @@
       <c r="J2">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K2">
+        <v>0</v>
+      </c>
+      <c r="L2">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -793,7 +854,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -825,7 +886,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -857,7 +918,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="6" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -889,7 +950,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -921,7 +982,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="8" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -953,7 +1014,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -985,7 +1046,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1017,7 +1078,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1049,7 +1110,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1081,7 +1142,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1113,7 +1174,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1145,7 +1206,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1177,7 +1238,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1209,7 +1270,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1241,7 +1302,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1273,7 +1334,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1304,8 +1365,11 @@
       <c r="J19">
         <v>5</v>
       </c>
-    </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="M19">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1336,8 +1400,17 @@
       <c r="J20">
         <v>0</v>
       </c>
-    </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K20">
+        <v>0</v>
+      </c>
+      <c r="L20">
+        <v>3</v>
+      </c>
+      <c r="M20">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1369,7 +1442,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1401,7 +1474,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1433,7 +1506,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1465,7 +1538,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="25" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -1497,7 +1570,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -1528,8 +1601,14 @@
       <c r="J26">
         <v>2</v>
       </c>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K26">
+        <v>2</v>
+      </c>
+      <c r="L26">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -1561,7 +1640,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -1593,7 +1672,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -1625,7 +1704,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -1657,7 +1736,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -1689,7 +1768,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -1721,7 +1800,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -1753,7 +1832,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -1785,7 +1864,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="35" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -1817,7 +1896,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="36" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -1849,7 +1928,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="37" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -1881,7 +1960,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -1912,8 +1991,14 @@
       <c r="J38">
         <v>2</v>
       </c>
-    </row>
-    <row r="39" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K38">
+        <v>4</v>
+      </c>
+      <c r="L38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -1945,7 +2030,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="40" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -1977,7 +2062,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="41" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2009,7 +2094,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="42" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2040,8 +2125,17 @@
       <c r="J42">
         <v>4</v>
       </c>
-    </row>
-    <row r="43" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="K42">
+        <v>0</v>
+      </c>
+      <c r="L42">
+        <v>0</v>
+      </c>
+      <c r="M42">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2073,7 +2167,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="44" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2105,7 +2199,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="45" spans="1:10" x14ac:dyDescent="0.3">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
         <v>43</v>
       </c>
@@ -2135,6 +2229,211 @@
       </c>
       <c r="J45">
         <v>4</v>
+      </c>
+      <c r="K45">
+        <v>0</v>
+      </c>
+      <c r="L45">
+        <v>0</v>
+      </c>
+      <c r="M45">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>105</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="C46">
+        <v>0</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>3</v>
+      </c>
+      <c r="F46">
+        <v>2</v>
+      </c>
+      <c r="G46">
+        <v>4</v>
+      </c>
+      <c r="H46">
+        <v>0</v>
+      </c>
+      <c r="I46">
+        <v>2</v>
+      </c>
+      <c r="J46">
+        <v>0</v>
+      </c>
+      <c r="K46">
+        <v>3</v>
+      </c>
+      <c r="L46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>99</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="C47">
+        <v>1</v>
+      </c>
+      <c r="D47">
+        <v>2</v>
+      </c>
+      <c r="E47">
+        <v>2</v>
+      </c>
+      <c r="F47">
+        <v>1</v>
+      </c>
+      <c r="G47">
+        <v>3</v>
+      </c>
+      <c r="H47">
+        <v>3</v>
+      </c>
+      <c r="I47">
+        <v>2</v>
+      </c>
+      <c r="J47">
+        <v>4</v>
+      </c>
+      <c r="K47">
+        <v>2</v>
+      </c>
+      <c r="L47">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>100</v>
+      </c>
+      <c r="B48" s="1" t="s">
+        <v>104</v>
+      </c>
+      <c r="C48">
+        <v>2</v>
+      </c>
+      <c r="D48">
+        <v>4</v>
+      </c>
+      <c r="E48">
+        <v>1</v>
+      </c>
+      <c r="F48">
+        <v>1</v>
+      </c>
+      <c r="G48">
+        <v>0</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>0</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>3</v>
+      </c>
+      <c r="L48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
+        <v>106</v>
+      </c>
+      <c r="B49" s="1" t="s">
+        <v>107</v>
+      </c>
+      <c r="C49">
+        <v>5</v>
+      </c>
+      <c r="D49">
+        <v>0</v>
+      </c>
+      <c r="E49">
+        <v>0</v>
+      </c>
+      <c r="F49">
+        <v>5</v>
+      </c>
+      <c r="G49">
+        <v>0</v>
+      </c>
+      <c r="H49">
+        <v>5</v>
+      </c>
+      <c r="I49">
+        <v>0</v>
+      </c>
+      <c r="J49">
+        <v>5</v>
+      </c>
+      <c r="K49">
+        <v>0</v>
+      </c>
+      <c r="L49">
+        <v>0</v>
+      </c>
+      <c r="M49">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>108</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>110</v>
+      </c>
+      <c r="C50">
+        <v>0</v>
+      </c>
+      <c r="D50">
+        <v>1</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>1</v>
+      </c>
+      <c r="G50">
+        <v>5</v>
+      </c>
+      <c r="H50">
+        <v>0</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>1</v>
+      </c>
+      <c r="L50">
+        <v>3</v>
+      </c>
+      <c r="M50">
+        <v>0</v>
       </c>
     </row>
   </sheetData>
@@ -2183,10 +2482,15 @@
     <hyperlink ref="B5" r:id="rId42"/>
     <hyperlink ref="B6" r:id="rId43"/>
     <hyperlink ref="B7" r:id="rId44"/>
+    <hyperlink ref="B46" r:id="rId45"/>
+    <hyperlink ref="B47" r:id="rId46"/>
+    <hyperlink ref="B48" r:id="rId47"/>
+    <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <tableParts count="1">
-    <tablePart r:id="rId45"/>
+    <tablePart r:id="rId50"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
suite le monstre et la fille
</commit_message>
<xml_diff>
--- a/musiques.xlsx
+++ b/musiques.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="6708" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="9108" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="115" uniqueCount="115">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="124" uniqueCount="124">
   <si>
     <t>army of doom</t>
   </si>
@@ -301,9 +301,6 @@
     <t>https://www.youtube.com/watch?v=z4-6Shvg8js</t>
   </si>
   <si>
-    <t>regard en arrierre</t>
-  </si>
-  <si>
     <t>Epilogue : beginning</t>
   </si>
   <si>
@@ -313,9 +310,6 @@
     <t>https://www.youtube.com/watch?v=TYevEJ6y7Uo</t>
   </si>
   <si>
-    <t>regard en avant</t>
-  </si>
-  <si>
     <t>https://www.youtube.com/watch?v=08XIghnIjWs</t>
   </si>
   <si>
@@ -359,6 +353,39 @@
   </si>
   <si>
     <t xml:space="preserve"> </t>
+  </si>
+  <si>
+    <t>la crise</t>
+  </si>
+  <si>
+    <t>en arrierre</t>
+  </si>
+  <si>
+    <t>en avant</t>
+  </si>
+  <si>
+    <t>quantum slash</t>
+  </si>
+  <si>
+    <t>Alice madness returns</t>
+  </si>
+  <si>
+    <t>simplicity</t>
+  </si>
+  <si>
+    <t>regrets</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=do26kpR3hT0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=j_dS5qIAsC0</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=qPL5gh8OxCw</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/watch?v=3kWR2HmNakQ</t>
   </si>
 </sst>
 </file>
@@ -409,16 +436,21 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="3">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1" applyAlignment="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Lien hypertexte" xfId="1" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="2">
+  <dxfs count="3">
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+    </dxf>
     <dxf>
       <fill>
         <patternFill patternType="solid">
@@ -451,9 +483,9 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:S49">
-  <autoFilter ref="A1:S49"/>
-  <tableColumns count="19">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:T53" headerRowDxfId="0">
+  <autoFilter ref="A1:T53"/>
+  <tableColumns count="20">
     <tableColumn id="1" name="titre" totalsRowLabel="Total"/>
     <tableColumn id="7" name="Lien"/>
     <tableColumn id="2" name="dark"/>
@@ -463,16 +495,17 @@
     <tableColumn id="8" name="perturbant"/>
     <tableColumn id="9" name="aventure"/>
     <tableColumn id="10" name="mysterieux"/>
-    <tableColumn id="12" name="regard en arrierre"/>
-    <tableColumn id="13" name="regard en avant"/>
+    <tableColumn id="12" name="en arrierre"/>
+    <tableColumn id="13" name="en avant"/>
     <tableColumn id="14" name="intense"/>
-    <tableColumn id="18" name=" " dataDxfId="0"/>
+    <tableColumn id="18" name=" " dataDxfId="2"/>
     <tableColumn id="15" name="ambiance"/>
     <tableColumn id="16" name="emotion"/>
     <tableColumn id="5" name="action"/>
     <tableColumn id="19" name="  " dataDxfId="1"/>
     <tableColumn id="17" name="révolte"/>
     <tableColumn id="20" name="posthumain" totalsRowFunction="sum"/>
+    <tableColumn id="11" name="la crise"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium11" showFirstColumn="1" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -765,10 +798,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:S49"/>
+  <dimension ref="A1:T53"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="A43" sqref="A43:XFD43"/>
+      <selection activeCell="S4" sqref="S4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -780,73 +813,76 @@
     <col min="7" max="7" width="11.5546875" customWidth="1"/>
     <col min="8" max="8" width="10.109375" customWidth="1"/>
     <col min="9" max="9" width="11.5546875" customWidth="1"/>
-    <col min="10" max="10" width="13.109375" customWidth="1"/>
-    <col min="11" max="11" width="16.6640625" customWidth="1"/>
+    <col min="10" max="10" width="9.33203125" customWidth="1"/>
+    <col min="11" max="11" width="8.88671875" customWidth="1"/>
     <col min="13" max="13" width="2.33203125" style="2" customWidth="1"/>
     <col min="17" max="17" width="2.44140625" style="2" customWidth="1"/>
     <col min="19" max="19" width="11.5546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A1" t="s">
+    <row r="1" spans="1:20" s="3" customFormat="1" x14ac:dyDescent="0.3">
+      <c r="A1" s="3" t="s">
         <v>51</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B1" s="3" t="s">
         <v>50</v>
       </c>
-      <c r="C1" t="s">
+      <c r="C1" s="3" t="s">
         <v>43</v>
       </c>
-      <c r="D1" t="s">
+      <c r="D1" s="3" t="s">
         <v>45</v>
       </c>
-      <c r="E1" t="s">
+      <c r="E1" s="3" t="s">
         <v>44</v>
       </c>
-      <c r="F1" t="s">
+      <c r="F1" s="3" t="s">
         <v>46</v>
       </c>
-      <c r="G1" t="s">
+      <c r="G1" s="3" t="s">
         <v>47</v>
       </c>
-      <c r="H1" t="s">
+      <c r="H1" s="3" t="s">
         <v>48</v>
       </c>
-      <c r="I1" t="s">
+      <c r="I1" s="3" t="s">
         <v>49</v>
       </c>
-      <c r="J1" t="s">
-        <v>95</v>
-      </c>
-      <c r="K1" t="s">
-        <v>99</v>
-      </c>
-      <c r="L1" t="s">
+      <c r="J1" s="3" t="s">
+        <v>114</v>
+      </c>
+      <c r="K1" s="3" t="s">
+        <v>115</v>
+      </c>
+      <c r="L1" s="3" t="s">
+        <v>109</v>
+      </c>
+      <c r="M1" s="4" t="s">
+        <v>112</v>
+      </c>
+      <c r="N1" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="O1" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="P1" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="Q1" s="4" t="s">
         <v>111</v>
       </c>
-      <c r="M1" s="2" t="s">
-        <v>114</v>
-      </c>
-      <c r="N1" t="s">
-        <v>109</v>
-      </c>
-      <c r="O1" t="s">
+      <c r="R1" s="3" t="s">
         <v>110</v>
       </c>
-      <c r="P1" t="s">
-        <v>108</v>
-      </c>
-      <c r="Q1" s="2" t="s">
+      <c r="S1" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="T1" s="3" t="s">
         <v>113</v>
       </c>
-      <c r="R1" t="s">
-        <v>112</v>
-      </c>
-      <c r="S1" t="s">
-        <v>106</v>
-      </c>
-    </row>
-    <row r="2" spans="1:19" x14ac:dyDescent="0.3">
+    </row>
+    <row r="2" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A2" t="s">
         <v>0</v>
       </c>
@@ -899,7 +935,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="3" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A3" t="s">
         <v>1</v>
       </c>
@@ -952,7 +988,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="4" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A4" t="s">
         <v>2</v>
       </c>
@@ -1004,8 +1040,11 @@
       <c r="S4">
         <v>3</v>
       </c>
-    </row>
-    <row r="5" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T4">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="5" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A5" t="s">
         <v>3</v>
       </c>
@@ -1057,8 +1096,11 @@
       <c r="S5">
         <v>2</v>
       </c>
-    </row>
-    <row r="6" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T5">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="6" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A6" t="s">
         <v>4</v>
       </c>
@@ -1111,7 +1153,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="7" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A7" t="s">
         <v>5</v>
       </c>
@@ -1163,8 +1205,11 @@
       <c r="S7">
         <v>0</v>
       </c>
-    </row>
-    <row r="8" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T7">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A8" t="s">
         <v>6</v>
       </c>
@@ -1217,7 +1262,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="9" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="9" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A9" t="s">
         <v>7</v>
       </c>
@@ -1270,7 +1315,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="10" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="10" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A10" t="s">
         <v>8</v>
       </c>
@@ -1322,8 +1367,11 @@
       <c r="S10">
         <v>0</v>
       </c>
-    </row>
-    <row r="11" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T10">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A11" t="s">
         <v>9</v>
       </c>
@@ -1373,7 +1421,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="12" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="12" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A12" t="s">
         <v>10</v>
       </c>
@@ -1423,7 +1471,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="13" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="13" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A13" t="s">
         <v>11</v>
       </c>
@@ -1473,7 +1521,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="14" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="14" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A14" t="s">
         <v>12</v>
       </c>
@@ -1525,8 +1573,11 @@
       <c r="S14">
         <v>0</v>
       </c>
-    </row>
-    <row r="15" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T14">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A15" t="s">
         <v>13</v>
       </c>
@@ -1558,7 +1609,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="16" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="16" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A16" t="s">
         <v>14</v>
       </c>
@@ -1608,7 +1659,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="17" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="17" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A17" t="s">
         <v>15</v>
       </c>
@@ -1640,7 +1691,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="18" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="18" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A18" t="s">
         <v>16</v>
       </c>
@@ -1690,7 +1741,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="19" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="19" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -1731,7 +1782,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="20" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="20" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A20" t="s">
         <v>18</v>
       </c>
@@ -1784,7 +1835,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="21" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="21" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A21" t="s">
         <v>19</v>
       </c>
@@ -1837,7 +1888,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="22" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
         <v>20</v>
       </c>
@@ -1890,7 +1941,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="23" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="23" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A23" t="s">
         <v>21</v>
       </c>
@@ -1940,7 +1991,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="24" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="24" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A24" t="s">
         <v>22</v>
       </c>
@@ -1990,7 +2041,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="25" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="25" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
         <v>23</v>
       </c>
@@ -2028,7 +2079,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="26" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A26" t="s">
         <v>24</v>
       </c>
@@ -2060,7 +2111,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="27" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A27" t="s">
         <v>25</v>
       </c>
@@ -2088,11 +2139,35 @@
       <c r="I27">
         <v>0</v>
       </c>
+      <c r="J27">
+        <v>0</v>
+      </c>
+      <c r="K27">
+        <v>3</v>
+      </c>
       <c r="L27">
         <v>2</v>
       </c>
-    </row>
-    <row r="28" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N27">
+        <v>2</v>
+      </c>
+      <c r="O27">
+        <v>5</v>
+      </c>
+      <c r="P27">
+        <v>0</v>
+      </c>
+      <c r="R27">
+        <v>0</v>
+      </c>
+      <c r="S27">
+        <v>2</v>
+      </c>
+      <c r="T27">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="28" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A28" t="s">
         <v>26</v>
       </c>
@@ -2120,11 +2195,35 @@
       <c r="I28">
         <v>2</v>
       </c>
+      <c r="J28">
+        <v>0</v>
+      </c>
+      <c r="K28">
+        <v>0</v>
+      </c>
       <c r="L28">
         <v>1</v>
       </c>
-    </row>
-    <row r="29" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N28">
+        <v>2</v>
+      </c>
+      <c r="O28">
+        <v>5</v>
+      </c>
+      <c r="P28">
+        <v>0</v>
+      </c>
+      <c r="R28">
+        <v>0</v>
+      </c>
+      <c r="S28">
+        <v>0</v>
+      </c>
+      <c r="T28">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="29" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A29" t="s">
         <v>27</v>
       </c>
@@ -2174,7 +2273,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="30" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="30" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A30" t="s">
         <v>28</v>
       </c>
@@ -2224,7 +2323,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="31" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="31" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A31" t="s">
         <v>29</v>
       </c>
@@ -2256,7 +2355,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="32" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="32" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A32" t="s">
         <v>30</v>
       </c>
@@ -2284,11 +2383,35 @@
       <c r="I32">
         <v>3</v>
       </c>
+      <c r="J32">
+        <v>5</v>
+      </c>
+      <c r="K32">
+        <v>3</v>
+      </c>
       <c r="L32">
         <v>3</v>
       </c>
-    </row>
-    <row r="33" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N32">
+        <v>5</v>
+      </c>
+      <c r="O32">
+        <v>5</v>
+      </c>
+      <c r="P32">
+        <v>2</v>
+      </c>
+      <c r="R32">
+        <v>1</v>
+      </c>
+      <c r="S32">
+        <v>0</v>
+      </c>
+      <c r="T32">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="33" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A33" t="s">
         <v>31</v>
       </c>
@@ -2338,7 +2461,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="34" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="34" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A34" t="s">
         <v>32</v>
       </c>
@@ -2388,7 +2511,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="35" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="35" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A35" t="s">
         <v>33</v>
       </c>
@@ -2441,7 +2564,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="36" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="36" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A36" t="s">
         <v>34</v>
       </c>
@@ -2494,7 +2617,7 @@
         <v>3</v>
       </c>
     </row>
-    <row r="37" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="37" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A37" t="s">
         <v>35</v>
       </c>
@@ -2544,7 +2667,7 @@
         <v>0</v>
       </c>
     </row>
-    <row r="38" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="38" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A38" t="s">
         <v>36</v>
       </c>
@@ -2594,7 +2717,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="39" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="39" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A39" t="s">
         <v>37</v>
       </c>
@@ -2622,11 +2745,32 @@
       <c r="I39">
         <v>0</v>
       </c>
+      <c r="J39">
+        <v>5</v>
+      </c>
+      <c r="K39">
+        <v>0</v>
+      </c>
       <c r="L39">
         <v>1</v>
       </c>
-    </row>
-    <row r="40" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N39">
+        <v>3</v>
+      </c>
+      <c r="O39">
+        <v>5</v>
+      </c>
+      <c r="P39">
+        <v>0</v>
+      </c>
+      <c r="R39">
+        <v>0</v>
+      </c>
+      <c r="S39">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="40" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A40" t="s">
         <v>38</v>
       </c>
@@ -2658,7 +2802,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="41" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="41" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A41" t="s">
         <v>39</v>
       </c>
@@ -2699,7 +2843,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="42" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="42" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A42" t="s">
         <v>40</v>
       </c>
@@ -2731,7 +2875,7 @@
         <v>4</v>
       </c>
     </row>
-    <row r="43" spans="1:19" x14ac:dyDescent="0.3">
+    <row r="43" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A43" t="s">
         <v>41</v>
       </c>
@@ -2759,11 +2903,35 @@
       <c r="I43">
         <v>3</v>
       </c>
+      <c r="J43">
+        <v>5</v>
+      </c>
+      <c r="K43">
+        <v>2</v>
+      </c>
       <c r="L43">
         <v>2</v>
       </c>
-    </row>
-    <row r="44" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="N43">
+        <v>5</v>
+      </c>
+      <c r="O43">
+        <v>4</v>
+      </c>
+      <c r="P43">
+        <v>1</v>
+      </c>
+      <c r="R43">
+        <v>0</v>
+      </c>
+      <c r="S43">
+        <v>0</v>
+      </c>
+      <c r="T43">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="44" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A44" t="s">
         <v>42</v>
       </c>
@@ -2800,181 +2968,238 @@
       <c r="L44">
         <v>4</v>
       </c>
+      <c r="N44">
+        <v>5</v>
+      </c>
+      <c r="O44">
+        <v>4</v>
+      </c>
+      <c r="P44">
+        <v>4</v>
+      </c>
+      <c r="R44">
+        <v>1</v>
+      </c>
       <c r="S44">
         <v>3</v>
       </c>
-    </row>
-    <row r="45" spans="1:19" x14ac:dyDescent="0.3">
+      <c r="T44">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="45" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A45" t="s">
+        <v>100</v>
+      </c>
+      <c r="B45" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="C45">
+        <v>0</v>
+      </c>
+      <c r="D45">
+        <v>2</v>
+      </c>
+      <c r="E45">
+        <v>3</v>
+      </c>
+      <c r="F45">
+        <v>4</v>
+      </c>
+      <c r="G45">
+        <v>0</v>
+      </c>
+      <c r="H45">
+        <v>2</v>
+      </c>
+      <c r="I45">
+        <v>0</v>
+      </c>
+      <c r="J45">
+        <v>3</v>
+      </c>
+      <c r="K45">
+        <v>3</v>
+      </c>
+      <c r="L45">
+        <v>2</v>
+      </c>
+      <c r="N45">
+        <v>0</v>
+      </c>
+      <c r="O45">
+        <v>5</v>
+      </c>
+      <c r="P45">
+        <v>2</v>
+      </c>
+      <c r="R45">
+        <v>0</v>
+      </c>
+      <c r="S45">
+        <v>0</v>
+      </c>
+      <c r="T45">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="46" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A46" t="s">
+        <v>95</v>
+      </c>
+      <c r="B46" s="1" t="s">
+        <v>98</v>
+      </c>
+      <c r="C46">
+        <v>1</v>
+      </c>
+      <c r="D46">
+        <v>2</v>
+      </c>
+      <c r="E46">
+        <v>2</v>
+      </c>
+      <c r="F46">
+        <v>3</v>
+      </c>
+      <c r="G46">
+        <v>3</v>
+      </c>
+      <c r="H46">
+        <v>2</v>
+      </c>
+      <c r="I46">
+        <v>4</v>
+      </c>
+      <c r="J46">
+        <v>2</v>
+      </c>
+      <c r="K46">
+        <v>5</v>
+      </c>
+      <c r="L46">
+        <v>1</v>
+      </c>
+      <c r="N46">
+        <v>4</v>
+      </c>
+      <c r="O46">
+        <v>4</v>
+      </c>
+      <c r="P46">
+        <v>0</v>
+      </c>
+      <c r="R46">
+        <v>0</v>
+      </c>
+      <c r="S46">
+        <v>0</v>
+      </c>
+      <c r="T46">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="47" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A47" t="s">
+        <v>96</v>
+      </c>
+      <c r="B47" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="C47">
+        <v>2</v>
+      </c>
+      <c r="D47">
+        <v>4</v>
+      </c>
+      <c r="E47">
+        <v>1</v>
+      </c>
+      <c r="F47">
+        <v>0</v>
+      </c>
+      <c r="G47">
+        <v>0</v>
+      </c>
+      <c r="H47">
+        <v>0</v>
+      </c>
+      <c r="I47">
+        <v>0</v>
+      </c>
+      <c r="J47">
+        <v>3</v>
+      </c>
+      <c r="K47">
+        <v>0</v>
+      </c>
+      <c r="L47">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A48" t="s">
+        <v>101</v>
+      </c>
+      <c r="B48" s="1" t="s">
         <v>102</v>
       </c>
-      <c r="B45" s="1" t="s">
-        <v>98</v>
-      </c>
-      <c r="C45">
-        <v>0</v>
-      </c>
-      <c r="D45">
-        <v>2</v>
-      </c>
-      <c r="E45">
-        <v>3</v>
-      </c>
-      <c r="F45">
-        <v>4</v>
-      </c>
-      <c r="G45">
-        <v>0</v>
-      </c>
-      <c r="H45">
-        <v>2</v>
-      </c>
-      <c r="I45">
-        <v>0</v>
-      </c>
-      <c r="J45">
-        <v>3</v>
-      </c>
-      <c r="K45">
-        <v>3</v>
-      </c>
-      <c r="L45">
-        <v>2</v>
-      </c>
-    </row>
-    <row r="46" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A46" t="s">
-        <v>96</v>
-      </c>
-      <c r="B46" s="1" t="s">
-        <v>100</v>
-      </c>
-      <c r="C46">
-        <v>1</v>
-      </c>
-      <c r="D46">
-        <v>2</v>
-      </c>
-      <c r="E46">
-        <v>2</v>
-      </c>
-      <c r="F46">
-        <v>3</v>
-      </c>
-      <c r="G46">
-        <v>3</v>
-      </c>
-      <c r="H46">
-        <v>2</v>
-      </c>
-      <c r="I46">
-        <v>4</v>
-      </c>
-      <c r="J46">
-        <v>2</v>
-      </c>
-      <c r="K46">
-        <v>5</v>
-      </c>
-      <c r="L46">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="47" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A47" t="s">
-        <v>97</v>
-      </c>
-      <c r="B47" s="1" t="s">
-        <v>101</v>
-      </c>
-      <c r="C47">
-        <v>2</v>
-      </c>
-      <c r="D47">
-        <v>4</v>
-      </c>
-      <c r="E47">
-        <v>1</v>
-      </c>
-      <c r="F47">
-        <v>0</v>
-      </c>
-      <c r="G47">
-        <v>0</v>
-      </c>
-      <c r="H47">
-        <v>0</v>
-      </c>
-      <c r="I47">
-        <v>0</v>
-      </c>
-      <c r="J47">
-        <v>3</v>
-      </c>
-      <c r="K47">
-        <v>0</v>
-      </c>
-      <c r="L47">
-        <v>1</v>
-      </c>
-    </row>
-    <row r="48" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A48" t="s">
+      <c r="C48">
+        <v>5</v>
+      </c>
+      <c r="D48">
+        <v>0</v>
+      </c>
+      <c r="E48">
+        <v>0</v>
+      </c>
+      <c r="F48">
+        <v>0</v>
+      </c>
+      <c r="G48">
+        <v>5</v>
+      </c>
+      <c r="H48">
+        <v>0</v>
+      </c>
+      <c r="I48">
+        <v>5</v>
+      </c>
+      <c r="J48">
+        <v>0</v>
+      </c>
+      <c r="K48">
+        <v>0</v>
+      </c>
+      <c r="L48">
+        <v>5</v>
+      </c>
+      <c r="N48">
+        <v>4</v>
+      </c>
+      <c r="O48">
+        <v>3</v>
+      </c>
+      <c r="P48">
+        <v>5</v>
+      </c>
+      <c r="R48">
+        <v>2</v>
+      </c>
+      <c r="S48">
+        <v>5</v>
+      </c>
+      <c r="T48">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="49" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A49" t="s">
         <v>103</v>
       </c>
-      <c r="B48" s="1" t="s">
-        <v>104</v>
-      </c>
-      <c r="C48">
-        <v>5</v>
-      </c>
-      <c r="D48">
-        <v>0</v>
-      </c>
-      <c r="E48">
-        <v>0</v>
-      </c>
-      <c r="F48">
-        <v>0</v>
-      </c>
-      <c r="G48">
-        <v>5</v>
-      </c>
-      <c r="H48">
-        <v>0</v>
-      </c>
-      <c r="I48">
-        <v>5</v>
-      </c>
-      <c r="J48">
-        <v>0</v>
-      </c>
-      <c r="K48">
-        <v>0</v>
-      </c>
-      <c r="L48">
-        <v>5</v>
-      </c>
-      <c r="N48">
-        <v>4</v>
-      </c>
-      <c r="O48">
-        <v>3</v>
-      </c>
-      <c r="P48">
-        <v>5</v>
-      </c>
-      <c r="S48">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="49" spans="1:19" x14ac:dyDescent="0.3">
-      <c r="A49" t="s">
+      <c r="B49" s="1" t="s">
         <v>105</v>
       </c>
-      <c r="B49" s="1" t="s">
-        <v>107</v>
-      </c>
       <c r="C49">
         <v>0</v>
       </c>
@@ -3016,6 +3241,230 @@
       </c>
       <c r="S49">
         <v>0</v>
+      </c>
+    </row>
+    <row r="50" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A50" t="s">
+        <v>116</v>
+      </c>
+      <c r="B50" s="1" t="s">
+        <v>120</v>
+      </c>
+      <c r="C50">
+        <v>3</v>
+      </c>
+      <c r="D50">
+        <v>3</v>
+      </c>
+      <c r="E50">
+        <v>0</v>
+      </c>
+      <c r="F50">
+        <v>2</v>
+      </c>
+      <c r="G50">
+        <v>2</v>
+      </c>
+      <c r="H50">
+        <v>3</v>
+      </c>
+      <c r="I50">
+        <v>3</v>
+      </c>
+      <c r="J50">
+        <v>0</v>
+      </c>
+      <c r="K50">
+        <v>2</v>
+      </c>
+      <c r="L50">
+        <v>2</v>
+      </c>
+      <c r="N50">
+        <v>5</v>
+      </c>
+      <c r="O50">
+        <v>4</v>
+      </c>
+      <c r="P50">
+        <v>3</v>
+      </c>
+      <c r="R50">
+        <v>3</v>
+      </c>
+      <c r="S50">
+        <v>3</v>
+      </c>
+      <c r="T50">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="51" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A51" t="s">
+        <v>117</v>
+      </c>
+      <c r="B51" s="1" t="s">
+        <v>121</v>
+      </c>
+      <c r="C51">
+        <v>4</v>
+      </c>
+      <c r="D51">
+        <v>0</v>
+      </c>
+      <c r="E51">
+        <v>2</v>
+      </c>
+      <c r="F51">
+        <v>0</v>
+      </c>
+      <c r="G51">
+        <v>5</v>
+      </c>
+      <c r="H51">
+        <v>0</v>
+      </c>
+      <c r="I51">
+        <v>5</v>
+      </c>
+      <c r="J51">
+        <v>0</v>
+      </c>
+      <c r="K51">
+        <v>0</v>
+      </c>
+      <c r="L51">
+        <v>2</v>
+      </c>
+      <c r="N51">
+        <v>5</v>
+      </c>
+      <c r="O51">
+        <v>3</v>
+      </c>
+      <c r="P51">
+        <v>0</v>
+      </c>
+      <c r="R51">
+        <v>2</v>
+      </c>
+      <c r="S51">
+        <v>5</v>
+      </c>
+      <c r="T51">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="52" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A52" t="s">
+        <v>118</v>
+      </c>
+      <c r="B52" s="1" t="s">
+        <v>122</v>
+      </c>
+      <c r="C52">
+        <v>0</v>
+      </c>
+      <c r="D52">
+        <v>0</v>
+      </c>
+      <c r="E52">
+        <v>2</v>
+      </c>
+      <c r="F52">
+        <v>5</v>
+      </c>
+      <c r="G52">
+        <v>0</v>
+      </c>
+      <c r="H52">
+        <v>3</v>
+      </c>
+      <c r="I52">
+        <v>0</v>
+      </c>
+      <c r="J52">
+        <v>3</v>
+      </c>
+      <c r="K52">
+        <v>3</v>
+      </c>
+      <c r="L52">
+        <v>1</v>
+      </c>
+      <c r="N52">
+        <v>5</v>
+      </c>
+      <c r="O52">
+        <v>4</v>
+      </c>
+      <c r="P52">
+        <v>0</v>
+      </c>
+      <c r="R52">
+        <v>0</v>
+      </c>
+      <c r="S52">
+        <v>0</v>
+      </c>
+      <c r="T52">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="53" spans="1:20" x14ac:dyDescent="0.3">
+      <c r="A53" t="s">
+        <v>119</v>
+      </c>
+      <c r="B53" s="1" t="s">
+        <v>123</v>
+      </c>
+      <c r="C53">
+        <v>3</v>
+      </c>
+      <c r="D53">
+        <v>5</v>
+      </c>
+      <c r="E53">
+        <v>0</v>
+      </c>
+      <c r="F53">
+        <v>0</v>
+      </c>
+      <c r="G53">
+        <v>0</v>
+      </c>
+      <c r="H53">
+        <v>2</v>
+      </c>
+      <c r="I53">
+        <v>0</v>
+      </c>
+      <c r="J53">
+        <v>5</v>
+      </c>
+      <c r="K53">
+        <v>0</v>
+      </c>
+      <c r="L53">
+        <v>1</v>
+      </c>
+      <c r="N53">
+        <v>4</v>
+      </c>
+      <c r="O53">
+        <v>5</v>
+      </c>
+      <c r="P53">
+        <v>0</v>
+      </c>
+      <c r="R53">
+        <v>5</v>
+      </c>
+      <c r="S53">
+        <v>3</v>
+      </c>
+      <c r="T53">
+        <v>5</v>
       </c>
     </row>
   </sheetData>
@@ -3068,11 +3517,15 @@
     <hyperlink ref="B47" r:id="rId46"/>
     <hyperlink ref="B48" r:id="rId47"/>
     <hyperlink ref="B49" r:id="rId48"/>
+    <hyperlink ref="B50" r:id="rId49"/>
+    <hyperlink ref="B51" r:id="rId50"/>
+    <hyperlink ref="B52" r:id="rId51"/>
+    <hyperlink ref="B53" r:id="rId52"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId49"/>
+  <pageSetup paperSize="9" orientation="portrait" horizontalDpi="360" verticalDpi="360" r:id="rId53"/>
   <tableParts count="1">
-    <tablePart r:id="rId50"/>
+    <tablePart r:id="rId54"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
progres survivants de la crise
</commit_message>
<xml_diff>
--- a/musiques.xlsx
+++ b/musiques.xlsx
@@ -4,7 +4,7 @@
   <fileVersion appName="xl" lastEdited="6" lowestEdited="4" rupBuild="14420"/>
   <workbookPr filterPrivacy="1" defaultThemeVersion="124226"/>
   <bookViews>
-    <workbookView xWindow="240" yWindow="9108" windowWidth="14808" windowHeight="8016"/>
+    <workbookView xWindow="240" yWindow="9708" windowWidth="14808" windowHeight="8016"/>
   </bookViews>
   <sheets>
     <sheet name="Feuil1" sheetId="1" r:id="rId1"/>
@@ -449,9 +449,6 @@
   </cellStyles>
   <dxfs count="3">
     <dxf>
-      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-    </dxf>
-    <dxf>
       <fill>
         <patternFill patternType="solid">
           <fgColor indexed="64"/>
@@ -466,6 +463,9 @@
           <bgColor theme="0"/>
         </patternFill>
       </fill>
+    </dxf>
+    <dxf>
+      <alignment horizontal="general" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
     </dxf>
   </dxfs>
   <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleMedium9">
@@ -483,7 +483,7 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:T53" headerRowDxfId="0">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" id="1" name="Tableau1" displayName="Tableau1" ref="A1:T53" headerRowDxfId="2">
   <autoFilter ref="A1:T53"/>
   <tableColumns count="20">
     <tableColumn id="1" name="titre" totalsRowLabel="Total"/>
@@ -498,11 +498,11 @@
     <tableColumn id="12" name="en arrierre"/>
     <tableColumn id="13" name="en avant"/>
     <tableColumn id="14" name="intense"/>
-    <tableColumn id="18" name=" " dataDxfId="2"/>
+    <tableColumn id="18" name=" " dataDxfId="1"/>
     <tableColumn id="15" name="ambiance"/>
     <tableColumn id="16" name="emotion"/>
     <tableColumn id="5" name="action"/>
-    <tableColumn id="19" name="  " dataDxfId="1"/>
+    <tableColumn id="19" name="  " dataDxfId="0"/>
     <tableColumn id="17" name="révolte"/>
     <tableColumn id="20" name="posthumain" totalsRowFunction="sum"/>
     <tableColumn id="11" name="la crise"/>
@@ -800,8 +800,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:T53"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <selection activeCell="S4" sqref="S4"/>
+    <sheetView tabSelected="1" topLeftCell="A4" zoomScaleNormal="100" workbookViewId="0">
+      <selection activeCell="J26" sqref="J26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="8.88671875" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -1417,7 +1417,13 @@
       <c r="P11">
         <v>0</v>
       </c>
+      <c r="R11">
+        <v>0</v>
+      </c>
       <c r="S11">
+        <v>0</v>
+      </c>
+      <c r="T11">
         <v>0</v>
       </c>
     </row>
@@ -1887,6 +1893,9 @@
       <c r="S21">
         <v>0</v>
       </c>
+      <c r="T21">
+        <v>0</v>
+      </c>
     </row>
     <row r="22" spans="1:20" x14ac:dyDescent="0.3">
       <c r="A22" t="s">
@@ -1987,8 +1996,14 @@
       <c r="P23">
         <v>0</v>
       </c>
+      <c r="R23">
+        <v>0</v>
+      </c>
       <c r="S23">
         <v>2</v>
+      </c>
+      <c r="T23">
+        <v>5</v>
       </c>
     </row>
     <row r="24" spans="1:20" x14ac:dyDescent="0.3">
@@ -2107,8 +2122,32 @@
       <c r="I26">
         <v>0</v>
       </c>
+      <c r="J26">
+        <v>5</v>
+      </c>
+      <c r="K26">
+        <v>0</v>
+      </c>
       <c r="L26">
         <v>2</v>
+      </c>
+      <c r="N26">
+        <v>2</v>
+      </c>
+      <c r="O26">
+        <v>5</v>
+      </c>
+      <c r="P26">
+        <v>0</v>
+      </c>
+      <c r="R26">
+        <v>0</v>
+      </c>
+      <c r="S26">
+        <v>0</v>
+      </c>
+      <c r="T26">
+        <v>5</v>
       </c>
     </row>
     <row r="27" spans="1:20" x14ac:dyDescent="0.3">

</xml_diff>